<commit_message>
Creation app streamlit moyenne
</commit_message>
<xml_diff>
--- a/Tableau métriques/moyenne/2021_2022/Skill Corner/moyenne_pressure.xlsx
+++ b/Tableau métriques/moyenne/2021_2022/Skill Corner/moyenne_pressure.xlsx
@@ -1514,16 +1514,16 @@
         <v>913.7543772450674</v>
       </c>
       <c r="D32" t="n">
-        <v>0.546582916979982</v>
+        <v>0.5465829169799821</v>
       </c>
       <c r="E32" t="n">
-        <v>65.71851524998368</v>
+        <v>65.71851524998364</v>
       </c>
       <c r="F32" t="n">
         <v>37.00748049513097</v>
       </c>
       <c r="G32" t="n">
-        <v>831.9386842105263</v>
+        <v>831.9386842105264</v>
       </c>
       <c r="H32" t="n">
         <v>850.9688235294117</v>

</xml_diff>